<commit_message>
date field [issue with findaphd]
</commit_message>
<xml_diff>
--- a/PhD_Positions_2022-05-15.xlsx
+++ b/PhD_Positions_2022-05-15.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C113"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,10 +441,15 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Title</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Link</t>
         </is>
@@ -458,10 +463,15 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>about 13 hours ago</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>AI-based bone fracture detection and classification (PhD Scholarship)</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Australia/Ai-Based-Bone-Fracture-Detection-And-Classification-Ph-D-Scholarship-Queensland-University-Of-Technology=9tbhyLyt7BGUYQAlkGUTnw.html</t>
         </is>
@@ -475,10 +485,15 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>about 4 hours ago</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>Embedded Intelligence – Deep Learning Algorithms and Architectures for Efficient Hardware Implementation PhD Scholarship</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Australia/Embedded-Intelligence-Deep-Learning-Algorithms-And-Architectures-For-Efficient-Hardware-Implementation-Ph-D-Scholarship-University-Of-The-Sunshine-Coast=bycnUriD7BGUYAAlkGUTnw.html</t>
         </is>
@@ -492,10 +507,15 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>8 days ago</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>Grant-Funded Researcher (A) - Machine Vision</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Australia/Grant-Funded-Researcher-A-Machine-Vision-University-Of-Adelaide=b9CHoQ_37BGUYQAlkGUTnw.html</t>
         </is>
@@ -509,10 +529,15 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>about 1 month ago</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>Grant-Funded Researcher (A), Machine Vision</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Australia/Grant-Funded-Researcher-A-Machine-Vision-University-Of-Adelaide=yWW_uvq47BGUYQAlkGUTnw.html</t>
         </is>
@@ -526,10 +551,15 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>17 days ago</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>PhD Scholarship in Automated Decision-Making and Information Retrieval</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Australia/Ph-D-Scholarship-In-Automated-Decision-Making-And-Information-Retrieval-Rmit-University=wkWBqSy77BGUYQAlkGUTnw.html</t>
         </is>
@@ -543,10 +573,15 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>17 days ago</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
           <t>PhD Scholarship in Automated Decision-Making and Machine Learning</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Australia/Ph-D-Scholarship-In-Automated-Decision-Making-And-Machine-Learning-Rmit-University=kWxBmiy77BGUYQAlkGUTnw.html</t>
         </is>
@@ -560,10 +595,15 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>about 2 months ago</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>PhD Scholarship in Computer Vision for Medical Imaging</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Australia/Ph-D-Scholarship-In-Computer-Vision-For-Medical-Imaging-Rmit-University=kEc3fjuk7BGUYAAlkGUTnw.html</t>
         </is>
@@ -577,10 +617,15 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>17 days ago</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>PhD Scholarship in Systems for Automated Decision-Making</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Australia/Ph-D-Scholarship-In-Systems-For-Automated-Decision-Making-Rmit-University=KcJvvCy77BGUYQAlkGUTnw.html</t>
         </is>
@@ -594,10 +639,15 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>43 minutes ago</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
           <t>PhD Scholarships in Automated Decision-Making</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Australia/Ph-D-Scholarships-In-Automated-Decision-Making-Rmit-University=XT9ZPiu77BGUYQAlkGUTnw.html</t>
         </is>
@@ -611,10 +661,15 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>23 days ago</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
           <t>PhD scholarship: Machine Learning in Airport X-Ray Baggage Inspection</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Australia/Ph-D-Scholarship-Machine-Learning-In-Airport-X-Ray-Baggage-Inspection-Flinders-University=iDDRI0wXq3vcio75YDgbec.html</t>
         </is>
@@ -628,10 +683,15 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>about 12 hours ago</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>QUT-CSIRO PhD Scholarship in Deep Learning for Hyperspectral Image Classification</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Australia/Qut-Csiro-Ph-D-Scholarship-In-Deep-Learning-For-Hyperspectral-Image-Classification-Queensland-University-Of-Technology=Eq3qYYyu7BGUYQAlkGUTnw.html</t>
         </is>
@@ -645,10 +705,15 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>2 months ago</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
           <t>PhD Student - Department of Information Technology</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Belgium/Ph-D-Student-Department-Of-Information-Technology-Ghent-University=robqm0yk7BGUYAAlkGUTnw.html</t>
         </is>
@@ -662,10 +727,15 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>about 7 hours ago</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>PhD Stipend in Self-Supervised Learning for Decoding of Complex Signals (8-22010)</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Denmark/Ph-D-Stipend-In-Self-Supervised-Learning-For-Decoding-Of-Complex-Signals-8-22010-Aalborg-University=cu3L9oSs7BGUYQAlkGUTnw.html</t>
         </is>
@@ -679,10 +749,15 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>11 days ago</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
           <t>PhD Position F/M L∪M_INTERMOD: Cross-cognitive and trans-cognitive modelling of multimodal  biomarkers with artificial intelligence methods. Application to the unified language- union-memory framework (L∪M)</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-France/Ph-D-Position-F-M-L-M-Intermod-Cross-Cognitive-And-Trans-Cognitive-Modelling-Of-Multimodal-Biomarkers-With-Artificial-Intelligence-Methods-Application-To-The-Unified-Language-Union-Memory-Framework-L-M-Inria=pTp4q4bC7BGUYQAlkGUTnw.html</t>
         </is>
@@ -696,10 +771,15 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>11 days ago</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
           <t>PhD Position F/M Numerical methods using graphs neural networks for the analyses of interactions of cells</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-France/Ph-D-Position-F-M-Numerical-Methods-Using-Graphs-Neural-Networks-For-The-Analyses-Of-Interactions-Of-Cells-Inria=sidqnobC7BGUYQAlkGUTnw.html</t>
         </is>
@@ -713,10 +793,15 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>11 days ago</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
           <t>PhD Position F/M [DOCT2022-COMPO-EPIONE] Optimizing sequential treatment in head and neck squamous cell carcinoma (HNSCC): artificial intelligence based on real-life patient data to support medical decision-making</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-France/Ph-D-Position-F-M-Doct2022-Compo-Epione-Optimizing-Sequential-Treatment-In-Head-And-Neck-Squamous-Cell-Carcinoma-Hnscc-Artificial-Intelligence-Based-On-Real-Life-Patient-Data-To-Support-Medical-Decision-Making-Inria=a5gqDv677BGUYQAlkGUTnw.html</t>
         </is>
@@ -730,10 +815,15 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>17 days ago</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
           <t>PhD in Astrophysics</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-France/Ph-D-In-Astrophysics-University-Of-Bordeaux=sjeG4ILG7BGUYQAlkGUTnw.html</t>
         </is>
@@ -747,10 +837,15 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
+          <t>about 1 month ago</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
           <t>PhD in fluid mechanics. Turbulent convection: numerical modelling and physics-enhanced machine...</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-France/Ph-D-In-Fluid-Mechanics-Turbulent-Convection-Numerical-Modelling-And-Physics-Enhanced-Machine-Universit-Paris-Saclay=HPwl8qO77BGUYQAlkGUTnw.html</t>
         </is>
@@ -764,10 +859,15 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>PhD position at University of Caen, CNRS GREYC Laboratory on Frugal AI for image segmentation</t>
+          <t>about 2 months ago</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
+        <is>
+          <t>PhD position at University of Caen, CNRS GREYC Laboratory on "Frugal AI for image segmentation"</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-France/Ph-D-Position-At-University-Of-Caen-Cnrs-Greyc-Laboratory-On-Frugal-Ai-For-Image-Segmentation-Universit-De-Caen-Normandie=Qjw8PLSq7BGUYAAlkGUTnw.html</t>
         </is>
@@ -781,10 +881,15 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
+          <t>1 day ago</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
           <t>Doctoral or Postdoctoral Positions in the Machine Learning and Information Processing Group at TUM</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Germany/Doctoral-Or-Postdoctoral-Positions-In-The-Machine-Learning-And-Information-Processing-Group-At-Tum-Technical-University-Of-Munich=sighLY607BGUYQAlkGUTnw.html</t>
         </is>
@@ -798,10 +903,15 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
+          <t>about 9 hours ago</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
           <t>Doctoral positions</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Germany/Doctoral-Positions-Technische-Universit-t-M-nchen=p5oIVYfA7BGUYQAlkGUTnw.html</t>
         </is>
@@ -815,10 +925,15 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
+          <t>26 days ago</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
           <t>PhD Position - Application of Machine Learning to Ranking Exhaustive Enumerations of Molecular...</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Germany/Ph-D-Position-Application-Of-Machine-Learning-To-Ranking-Exhaustive-Enumerations-Of-Molecular-J-lich-Research-Centre-Fzj=OxU5Emm97BGUYQAlkGUTnw.html</t>
         </is>
@@ -832,10 +947,15 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
+          <t>12 days ago</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
           <t>PhD Position – Computational quantum many-body physics</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Germany/Ph-D-Position-Computational-Quantum-Many-Body-Physics-J-lich-Research-Centre-Fzj=BVnuwB7J7BGUYQAlkGUTnw.html</t>
         </is>
@@ -849,10 +969,15 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
+          <t>2 months ago</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
           <t>PhD Student (m/f/d)</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Germany/Ph-D-Student-M-F-D-Katholische-Universit-t-Eichst-tt-Ingolstadt=2Gz8V4qZ7BGUYAAlkGUTnw.html</t>
         </is>
@@ -866,10 +991,15 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
+          <t>12 days ago</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
           <t>PhD in genomic surveillance of airborne pathogens (f/m/x)</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Germany/Ph-D-In-Genomic-Surveillance-Of-Airborne-Pathogens-F-M-X-Helmholtz-Munich=yEXgsx7J7BGUYQAlkGUTnw.html</t>
         </is>
@@ -883,10 +1013,15 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>about 3 hours ago</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
           <t>PhD student (m/f/d)</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Germany/Ph-D-Student-M-F-D-Leibniz=WwTYTBag7BGUYAAlkGUTnw.html</t>
         </is>
@@ -900,10 +1035,15 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
+          <t>about 1 month ago</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
           <t>PhD student in Bioinformatics or Computational Biology</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Germany/Ph-D-Student-In-Bioinformatics-Or-Computational-Biology-Leibniz-Institute-Of-Plant-Biochemistry=Qh65xL6g7BGUYAAlkGUTnw.html</t>
         </is>
@@ -917,10 +1057,15 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
+          <t>about 2 months ago</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
           <t>PhD/Postdoc in High Performance Machine Learning (m/f/d)</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Germany/Ph-D-Postdoc-In-High-Performance-Machine-Learning-M-F-D-Friedrich-Schiller-University-Jena=l9PetZml7BGUYAAlkGUTnw.html</t>
         </is>
@@ -934,10 +1079,15 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
+          <t>about 2 months ago</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
           <t>Postdoc (optionally PhD) candidate in deep learning for analysis of bioimage data</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Germany/Postdoc-Optionally-Ph-D-Candidate-In-Deep-Learning-For-Analysis-Of-Bioimage-Data-Center-For-Molecular-Medicine-Cologne=yGuIEY8esd1vucD9GufZw7.html</t>
         </is>
@@ -951,10 +1101,15 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
+          <t>2 months ago</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
           <t>Postdoc (optionally PhD) candidate in deep learning for analysis of bioimage data</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Germany/Postdoc-Optionally-Ph-D-Candidate-In-Deep-Learning-For-Analysis-Of-Bioimage-Data-Data-Science-Of-Bioimages=UT4v_KWh7BGUYAAlkGUTnw.html</t>
         </is>
@@ -968,10 +1123,15 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
+          <t>2 months ago</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
           <t>Student Research Assistant(s) (m/f/d, approx. 40h/month)</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/jobs-in-Germany/Student-Research-Assistant-S-M-F-D-Approx-40h-Month-University-Of-T-bingen=U0K82XCO7BGUYAAlkGUTnw.html</t>
         </is>
@@ -983,12 +1143,13 @@
           <t>Ireland</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="B33" t="inlineStr"/>
+      <c r="C33" t="inlineStr">
         <is>
           <t>Fully Funded Research Masters Student Position in Deep Learning for Biomedical Applications</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>https://www.findaphd.com/phds/project/fully-funded-research-masters-student-position-in-deep-learning-for-biomedical-applications/?p144295</t>
         </is>
@@ -1000,12 +1161,13 @@
           <t>Ireland</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="B34" t="inlineStr"/>
+      <c r="C34" t="inlineStr">
         <is>
           <t>Using Machine Learning Techniques to Detect Emotional Traits and Mathematics Anxiety Levels From Game Data</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>https://www.findaphd.com/phds/project/using-machine-learning-techniques-to-detect-emotional-traits-and-mathematics-anxiety-levels-from-game-data/?p136342</t>
         </is>
@@ -1019,10 +1181,15 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
+          <t>12 days ago</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
           <t>Doctoral Candidate (PhD student) in Applied Artificial Intelligence and Machine Learning for...</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Luxembourg/Doctoral-Candidate-Ph-D-Student-In-Applied-Artificial-Intelligence-And-Machine-Learning-For-University-Of-Luxembourg=8CS5Ln3K7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1036,10 +1203,15 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
+          <t>29 days ago</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
           <t>Doctoral Candidate (PhD student) in Applied Artificial Intelligence and Machine Learning for...</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Luxembourg/Doctoral-Candidate-Ph-D-Student-In-Applied-Artificial-Intelligence-And-Machine-Learning-For-University-Of-Luxembourg=_Cv0Gw687BGUYQAlkGUTnw.html</t>
         </is>
@@ -1053,10 +1225,15 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
+          <t>about 2 months ago</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
           <t>PhD Candidates / Spontaneous Applications</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Luxembourg/Ph-D-Candidates-Spontaneous-Applications-University-Of-Luxembourg=pA-3oPyr7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1070,10 +1247,15 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
+          <t>about 2 months ago</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
           <t>Research Associates / Spontaneous Applications</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/jobs-in-Luxembourg/Research-Associates-Spontaneous-Applications-University-Of-Luxembourg=aUSLevyr7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1087,10 +1269,15 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
+          <t>2 months ago</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
           <t>3 PhD Positions in Computer Vision</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Netherlands/3-Ph-D-Positions-In-Computer-Vision-University-Of-Amsterdam-Uv-A=ISU1Hjyh7BGUYAAlkGUTnw.html</t>
         </is>
@@ -1104,10 +1291,15 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
+          <t>2 months ago</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
           <t>3 PhD Positions in Computer Vision</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Netherlands/3-Ph-D-Positions-In-Computer-Vision-University-Of-Amsterdam=f8ab23Kg7BGUYAAlkGUTnw.html</t>
         </is>
@@ -1121,10 +1313,15 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
+          <t>about 24 hours ago</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
           <t>5-year PhD position in Automated Detection and Synthesis of Facial Actions (1.0 FTE)</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Netherlands/5-Year-Ph-D-Position-In-Automated-Detection-And-Synthesis-Of-Facial-Actions-1-0-Fte-Utrecht-University=Q1VBe2HL7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1138,10 +1335,15 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
+          <t>about 2 months ago</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
           <t>BIOLab PhD Position 4/4 Deep learning and smart super-resolution microscopy</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="D42" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Netherlands/Bio-Lab-Ph-D-Position-4-4-Deep-Learning-And-Smart-Super-Resolution-Microscopy-Delft-University-Of-Technology=-HOXaQKp7BGUYAAlkGUTnw.html</t>
         </is>
@@ -1155,10 +1357,15 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
+          <t>about 14 hours ago</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
           <t>Multiple PhD Positions in Machine Learning</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="D43" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Netherlands/Multiple-Ph-D-Positions-In-Machine-Learning-University-Of-Amsterdam-Uv-A=MyVO_xPM7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1172,10 +1379,15 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
+          <t>5 days ago</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
           <t>Multiple PhD Positions in Machine Learning</t>
         </is>
       </c>
-      <c r="C44" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Netherlands/Multiple-Ph-D-Positions-In-Machine-Learning-University-Of-Amsterdam=fH2cjsnL7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1189,10 +1401,15 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
+          <t>24 days ago</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
           <t>PDEng student on Deep learning to detect bitmap artefacts</t>
         </is>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="D45" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Netherlands/Pd-Eng-Student-On-Deep-Learning-To-Detect-Bitmap-Artefacts-Eindhoven-University-Of-Technology-Tu-E=LH7fuPi17BGUYQAlkGUTnw.html</t>
         </is>
@@ -1206,10 +1423,15 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
+          <t>about 7 hours ago</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
           <t>PDEng student on Deep learning to detect bitmap artefacts</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Netherlands/Pd-Eng-Student-On-Deep-Learning-To-Detect-Bitmap-Artefacts-Eindhoven-University-Of-Technology=5wwaEt_17BGUYQAlkGUTnw.html</t>
         </is>
@@ -1223,10 +1445,15 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
+          <t>5 days ago</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
           <t>PhD Candidate in Conversational Artificial Intelligence for Business</t>
         </is>
       </c>
-      <c r="C47" t="inlineStr">
+      <c r="D47" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Netherlands/Ph-D-Candidate-In-Conversational-Artificial-Intelligence-For-Business-University-Of-Amsterdam=uwaBAJbL7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1240,10 +1467,15 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
+          <t>13 days ago</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
           <t>PhD Candidate: Interpretable Information Extraction for Disaster Relief (1.0 FTE)</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
+      <c r="D48" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Netherlands/Ph-D-Candidate-Interpretable-Information-Extraction-For-Disaster-Relief-1-0-Fte-Radboud-University=xc6rfqWr7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1257,10 +1489,15 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
+          <t>5 days ago</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
           <t>PhD Position in Computer Vision for Film Analysis and Production</t>
         </is>
       </c>
-      <c r="C49" t="inlineStr">
+      <c r="D49" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Netherlands/Ph-D-Position-In-Computer-Vision-For-Film-Analysis-And-Production-University-Of-Amsterdam=gl6jTsnL7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1274,10 +1511,15 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
+          <t>2 days ago</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
           <t>PhD Position in Conversational Search and Recommendation</t>
         </is>
       </c>
-      <c r="C50" t="inlineStr">
+      <c r="D50" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Netherlands/Ph-D-Position-In-Conversational-Search-And-Recommendation-University-Of-Amsterdam=qA-98oy57BGUYQAlkGUTnw.html</t>
         </is>
@@ -1291,10 +1533,15 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
+          <t>about 2 months ago</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
           <t>PhD Position in Machine Learning</t>
         </is>
       </c>
-      <c r="C51" t="inlineStr">
+      <c r="D51" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Netherlands/Ph-D-Position-In-Machine-Learning-University-Of-Amsterdam-Uv-A=vGUlEsKb7BGUYAAlkGUTnw.html</t>
         </is>
@@ -1308,10 +1555,15 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
+          <t>3 months ago</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
           <t>PhD candidate 'Machine learning for digital biomarkers of Parkinson’s disease'</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
+      <c r="D52" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Netherlands/Ph-D-Candidate-Machine-Learning-For-Digital-Biomarkers-Of-Parkinson-s-Disease-Radboud-University-Medical-Center-Radboudumc=8eiW1GaQ7BGUYAAlkGUTnw.html</t>
         </is>
@@ -1325,10 +1577,15 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
+          <t>4 days ago</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
           <t>PhD Candidate in Deep Learning for Face Image Quality Metrics</t>
         </is>
       </c>
-      <c r="C53" t="inlineStr">
+      <c r="D53" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Norway/Ph-D-Candidate-In-Deep-Learning-For-Face-Image-Quality-Metrics-Ntnu-Norwegian-University-Of-Science-And-Technology=s24aWqrQ7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1342,10 +1599,15 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
+          <t>about 10 hours ago</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
           <t>PhD Candidate on Video Quality Assessment and Enhancement for Medical Services</t>
         </is>
       </c>
-      <c r="C54" t="inlineStr">
+      <c r="D54" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Norway/Ph-D-Candidate-On-Video-Quality-Assessment-And-Enhancement-For-Medical-Services-Ntnu=xDx_qLHK7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1359,10 +1621,15 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
+          <t>11 days ago</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
           <t>PhD Candidate on Video Quality Assessment and Enhancement for Medical Services</t>
         </is>
       </c>
-      <c r="C55" t="inlineStr">
+      <c r="D55" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Norway/Ph-D-Candidate-On-Video-Quality-Assessment-And-Enhancement-For-Medical-Services-Ntnu-Norwegian-University-Of-Science-And-Technology=4XS4Ke3K7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1376,10 +1643,15 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
+          <t>11 days ago</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
           <t>PhD Fellow in Computer Science - Efficient distributed machine learning</t>
         </is>
       </c>
-      <c r="C56" t="inlineStr">
+      <c r="D56" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Norway/Ph-D-Fellow-In-Computer-Science-Efficient-Distributed-Machine-Learning-Ui-T-The-Arctic-University-Of-Norway=Rflp9F7L7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1393,10 +1665,15 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
+          <t>about 2 months ago</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
           <t>PhD position within machine learning for Zero-Shot Learning using Multimodal Sensors (ZSL++)</t>
         </is>
       </c>
-      <c r="C57" t="inlineStr">
+      <c r="D57" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Norway/Ph-D-Position-Within-Machine-Learning-For-Zero-Shot-Learning-Using-Multimodal-Sensors-Zsl-Norwegian-University-Of-Life-Sciences-Nmbu=Hawahl_v7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1410,10 +1687,15 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
+          <t>1 day ago</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
           <t>PhD-position</t>
         </is>
       </c>
-      <c r="C58" t="inlineStr">
+      <c r="D58" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Norway/Ph-D-Position-University-Of-Bergen=INBrBJHS7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1427,10 +1709,15 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
+          <t>about 15 hours ago</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
           <t>PhD-position</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
+      <c r="D59" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Norway/Ph-D-Position-University-Of-Bergen=TSFqBsbS7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1444,10 +1731,15 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
+          <t>about 1 month ago</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
           <t>Research Junior</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
+      <c r="D60" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/jobs-in-Poland/Research-Junior-Jagiellonian-University=UgI6fKW37BGUYQAlkGUTnw.html</t>
         </is>
@@ -1461,10 +1753,15 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
+          <t>1 day ago</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
           <t>Sano PhD Student - Project title: Deep Learning-based Surgical Robots</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
+      <c r="D61" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Poland/Sano-Ph-D-Student-Project-Title-Deep-Learning-Based-Surgical-Robots-Sano-Centre-For-Computational-Personalized-Medicine=yV4mvtDS7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1478,10 +1775,15 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
+          <t>24 days ago</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
           <t>International Selection Procedure for Hiring a PhD Researcher - Notice no. 7740/2022</t>
         </is>
       </c>
-      <c r="C62" t="inlineStr">
+      <c r="D62" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Portugal/International-Selection-Procedure-For-Hiring-A-Ph-D-Researcher-Notice-No-7740-2022-Instituto-De-Geografia-E-Ordenamento-Do-Territ-rio-Da-Universidade-De-Lisboa=NPzs5WvB7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1495,10 +1797,15 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
+          <t>about 1 hour ago</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
           <t>Refª: CITIN-2021-RHAQ-SCF-P08-PHD</t>
         </is>
       </c>
-      <c r="C63" t="inlineStr">
+      <c r="D63" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Portugal/Ref-Citin-2021-Rhaq-Scf-P08-Phd-Ci-Tin-Associa-o-Centro-De-Interface-Tecnol-gico-Industrial=qc66F6vT7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1512,10 +1819,15 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
+          <t>about 20 hours ago</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
           <t>Doctoral Researcher in mathematical analyis &amp; numerical analysis for models in machine learning</t>
         </is>
       </c>
-      <c r="C64" t="inlineStr">
+      <c r="D64" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Spain/Doctoral-Researcher-In-Mathematical-Analyis-Numerical-Analysis-For-Models-In-Machine-Learning-Technische-Universit-t-M-nchen=zi4fjkvA7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1529,10 +1841,15 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
+          <t>about 1 month ago</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
           <t>PI - PhD GRANTS IN ARTIFICIAL INTELLIGENCE FOR SMART MOBILITY</t>
         </is>
       </c>
-      <c r="C65" t="inlineStr">
+      <c r="D65" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Spain/Pi-Ph-D-Grants-In-Artificial-Intelligence-For-Smart-Mobility-University-Of-Deusto=rCWblTW37BGUYQAlkGUTnw.html</t>
         </is>
@@ -1546,10 +1863,15 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
+          <t>about 1 hour ago</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
           <t>Doctoral students in Automatic Control (PA2022/1498)</t>
         </is>
       </c>
-      <c r="C66" t="inlineStr">
+      <c r="D66" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Sweden/Doctoral-Students-In-Automatic-Control-Pa2022-1498-University-Of-Lund=VBH2MgfM7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1563,10 +1885,15 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
+          <t>about 23 hours ago</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
           <t>PhD student in Operation and maintenance with specialization in Industrial Artificial Intelligence and eMaintenance</t>
         </is>
       </c>
-      <c r="C67" t="inlineStr">
+      <c r="D67" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Sweden/Ph-D-Student-In-Operation-And-Maintenance-With-Specialization-In-Industrial-Artificial-Intelligence-And-E-Maintenance-Lulea-University-Of-Technology=btIpedC37BGUYQAlkGUTnw.html</t>
         </is>
@@ -1580,10 +1907,15 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
+          <t>about 1 hour ago</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
           <t>PhD student in Scientific Computing focusing on Deep Learning for Genetic Epidemiology</t>
         </is>
       </c>
-      <c r="C68" t="inlineStr">
+      <c r="D68" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Sweden/Ph-D-Student-In-Scientific-Computing-Focusing-On-Deep-Learning-For-Genetic-Epidemiology-Uppsala-University=xTMTAovG7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1597,10 +1929,15 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
+          <t>4 days ago</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
           <t>PhD student in computer graphics and machine learning</t>
         </is>
       </c>
-      <c r="C69" t="inlineStr">
+      <c r="D69" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Sweden/Ph-D-Student-In-Computer-Graphics-And-Machine-Learning-Link-ping-University=Dqud1Am77BGUYQAlkGUTnw.html</t>
         </is>
@@ -1614,10 +1951,15 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
+          <t>about 18 hours ago</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
           <t>PhD students in machine learning for image generation</t>
         </is>
       </c>
-      <c r="C70" t="inlineStr">
+      <c r="D70" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Sweden/Ph-D-Students-In-Machine-Learning-For-Image-Generation-Link-ping-University=ivtGNTDR7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1631,10 +1973,15 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
+          <t>about 12 hours ago</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
           <t>ENAC – PhD Student in Deep Domain Adaptation for Fleet Knowledge Transfer</t>
         </is>
       </c>
-      <c r="C71" t="inlineStr">
+      <c r="D71" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Switzerland/Enac-Ph-D-Student-In-Deep-Domain-Adaptation-For-Fleet-Knowledge-Transfer-Epfl=rpVntGSQ7BGUYAAlkGUTnw.html</t>
         </is>
@@ -1648,10 +1995,15 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
+          <t>about 12 hours ago</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
           <t>ENAC – PhD Student in Physics – Informed Deep Learning for System Condition Monitoring and Prediction</t>
         </is>
       </c>
-      <c r="C72" t="inlineStr">
+      <c r="D72" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Switzerland/Enac-Ph-D-Student-In-Physics-Informed-Deep-Learning-For-System-Condition-Monitoring-And-Prediction-Epfl=4OUEqGSQ7BGUYAAlkGUTnw.html</t>
         </is>
@@ -1665,10 +2017,15 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
+          <t>about 1 month ago</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
           <t>Multiple PhD Positions in Machine Learning for Healthcare (# of pos: 2)</t>
         </is>
       </c>
-      <c r="C73" t="inlineStr">
+      <c r="D73" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Switzerland/Multiple-Ph-D-Positions-In-Machine-Learning-For-Healthcare-Of-Pos-2-University-Of-Bern=NFFFAf607BGUYQAlkGUTnw.html</t>
         </is>
@@ -1682,10 +2039,15 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
+          <t>11 days ago</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
           <t>PhD Position</t>
         </is>
       </c>
-      <c r="C74" t="inlineStr">
+      <c r="D74" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Switzerland/Ph-D-Position-University-Of-Basel=XmyzGdrL7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1699,10 +2061,15 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
+          <t>about 2 months ago</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
           <t>PhD position in Physics-Informed Machine Learning for Cardiac Imaging</t>
         </is>
       </c>
-      <c r="C75" t="inlineStr">
+      <c r="D75" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Switzerland/Ph-D-Position-In-Physics-Informed-Machine-Learning-For-Cardiac-Imaging-Eth-Zurich=p-5-0J6q7BGUYAAlkGUTnw.html</t>
         </is>
@@ -1716,10 +2083,15 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
+          <t>about 2 months ago</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
           <t>PhD position in Physics-Informed Machine Learning for Cardiac Imaging</t>
         </is>
       </c>
-      <c r="C76" t="inlineStr">
+      <c r="D76" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Switzerland/Ph-D-Position-In-Physics-Informed-Machine-Learning-For-Cardiac-Imaging-Eth-Zurich=l1lsvHSs7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1733,10 +2105,15 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
+          <t>23 days ago</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
           <t>PhD student in surgical data science and computer vision</t>
         </is>
       </c>
-      <c r="C77" t="inlineStr">
+      <c r="D77" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Switzerland/Ph-D-Student-In-Surgical-Data-Science-And-Computer-Vision-University-Of-Zurich=jPpVU-uj7BGUYAAlkGUTnw.html</t>
         </is>
@@ -1750,10 +2127,15 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
+          <t>12 days ago</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
           <t>PhD student medical AR and computer vision</t>
         </is>
       </c>
-      <c r="C78" t="inlineStr">
+      <c r="D78" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-Switzerland/Ph-D-Student-Medical-Ar-And-Computer-Vision-University-Of-Zurich=TmUpTfuj7BGUYAAlkGUTnw.html</t>
         </is>
@@ -1767,10 +2149,15 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
+          <t>about 2 months ago</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
           <t>Research Assistant under Division of Science, Computer Science</t>
         </is>
       </c>
-      <c r="C79" t="inlineStr">
+      <c r="D79" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/jobs-in-United-Arab-Emirates/Research-Assistant-Under-Division-Of-Science-Computer-Science-New-York-University-Abu-Dhabi=yYOdukOn7BGUYAAlkGUTnw.html</t>
         </is>
@@ -1782,12 +2169,13 @@
           <t>United Kingdom</t>
         </is>
       </c>
-      <c r="B80" t="inlineStr">
+      <c r="B80" t="inlineStr"/>
+      <c r="C80" t="inlineStr">
         <is>
           <t>Automated Classification and Identification of Plant Specimens of the Royal Botanic Gardens Kew Using Imaging Processing, AI and Machine Learning</t>
         </is>
       </c>
-      <c r="C80" t="inlineStr">
+      <c r="D80" t="inlineStr">
         <is>
           <t>https://www.findaphd.com/phds/project/automated-classification-and-identification-of-plant-specimens-of-the-royal-botanic-gardens-kew-using-imaging-processing-ai-and-machine-learning/?p144571</t>
         </is>
@@ -1801,10 +2189,15 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
+          <t>3 months ago</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
           <t>Biological Sciences: Fully Funded PhD Scholarship: Novel machine-vision and deep-learning...</t>
         </is>
       </c>
-      <c r="C81" t="inlineStr">
+      <c r="D81" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-United-Kingdom/Biological-Sciences-Fully-Funded-Ph-D-Scholarship-Novel-Machine-Vision-And-Deep-Learning-Swansea-University=MZgaIMqN7BGUYAAlkGUTnw.html</t>
         </is>
@@ -1816,12 +2209,13 @@
           <t>United Kingdom</t>
         </is>
       </c>
-      <c r="B82" t="inlineStr">
+      <c r="B82" t="inlineStr"/>
+      <c r="C82" t="inlineStr">
         <is>
           <t>Data-Driven Defect Detection for Additive Manufacturing”</t>
         </is>
       </c>
-      <c r="C82" t="inlineStr">
+      <c r="D82" t="inlineStr">
         <is>
           <t>https://www.findaphd.com/phds/project/data-driven-defect-detection-for-additive-manufacturing/?p144423</t>
         </is>
@@ -1833,12 +2227,13 @@
           <t>United Kingdom</t>
         </is>
       </c>
-      <c r="B83" t="inlineStr">
+      <c r="B83" t="inlineStr"/>
+      <c r="C83" t="inlineStr">
         <is>
           <t>Deep Learning and Partial Differential Equations</t>
         </is>
       </c>
-      <c r="C83" t="inlineStr">
+      <c r="D83" t="inlineStr">
         <is>
           <t>https://www.findaphd.com/phds/project/deep-learning-and-partial-differential-equations/?p138769</t>
         </is>
@@ -1850,12 +2245,13 @@
           <t>United Kingdom</t>
         </is>
       </c>
-      <c r="B84" t="inlineStr">
+      <c r="B84" t="inlineStr"/>
+      <c r="C84" t="inlineStr">
         <is>
           <t>Discovery of high-temperature superconductors using Deep Learning</t>
         </is>
       </c>
-      <c r="C84" t="inlineStr">
+      <c r="D84" t="inlineStr">
         <is>
           <t>https://www.findaphd.com/phds/project/discovery-of-high-temperature-superconductors-using-deep-learning/?p140230</t>
         </is>
@@ -1867,12 +2263,13 @@
           <t>United Kingdom</t>
         </is>
       </c>
-      <c r="B85" t="inlineStr">
+      <c r="B85" t="inlineStr"/>
+      <c r="C85" t="inlineStr">
         <is>
           <t>Discovery of new materials for applications on glass using Deep Machine Learning and Data Analytics</t>
         </is>
       </c>
-      <c r="C85" t="inlineStr">
+      <c r="D85" t="inlineStr">
         <is>
           <t>https://www.findaphd.com/phds/project/discovery-of-new-materials-for-applications-on-glass-using-deep-machine-learning-and-data-analytics/?p142079</t>
         </is>
@@ -1884,12 +2281,13 @@
           <t>United Kingdom</t>
         </is>
       </c>
-      <c r="B86" t="inlineStr">
+      <c r="B86" t="inlineStr"/>
+      <c r="C86" t="inlineStr">
         <is>
           <t>Discovery of solid state electrolytes using Deep Learning</t>
         </is>
       </c>
-      <c r="C86" t="inlineStr">
+      <c r="D86" t="inlineStr">
         <is>
           <t>https://www.findaphd.com/phds/project/discovery-of-solid-state-electrolytes-using-deep-learning/?p140199</t>
         </is>
@@ -1903,10 +2301,15 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
+          <t>9 days ago</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
           <t>EPSRC DTP PhD Studentship: Building interpretable generative models of images</t>
         </is>
       </c>
-      <c r="C87" t="inlineStr">
+      <c r="D87" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-United-Kingdom/Epsrc-Dtp-Ph-D-Studentship-Building-Interpretable-Generative-Models-Of-Images-University-Of-Sussex=0uLygSrM7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1920,10 +2323,15 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
+          <t>5 days ago</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
           <t>EPSRC/BAE Systems INDUSTRIAL CASE PhD Studentship - Mitigation of Reinforcement Learning Algorithms in Changing Environments</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr">
+      <c r="D88" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-United-Kingdom/Epsrc-Bae-Systems-Industrial-Case-Ph-D-Studentship-Mitigation-Of-Reinforcement-Learning-Algorithms-In-Changing-Environments-The-University-Of-Manchester=Nv-i4HLQ7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1937,10 +2345,15 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
+          <t>3 months ago</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
           <t>Fully Funded PhD Scholarship: Novel Machine-vision and Deep-learning Applications to Assess the Welfare of Cleaner fFsh in the Salmon Industry</t>
         </is>
       </c>
-      <c r="C89" t="inlineStr">
+      <c r="D89" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-United-Kingdom/Fully-Funded-Ph-D-Scholarship-Novel-Machine-Vision-And-Deep-Learning-Applications-To-Assess-The-Welfare-Of-Cleaner-F-Fsh-In-The-Salmon-Industry-Swansea-University=G7RDo-mP7BGUYAAlkGUTnw.html</t>
         </is>
@@ -1954,10 +2367,15 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
+          <t>9 days ago</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
           <t>PhD Candidate on Video Quality Assessment and Enhancement for Medical Services</t>
         </is>
       </c>
-      <c r="C90" t="inlineStr">
+      <c r="D90" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-United-Kingdom/Ph-D-Candidate-On-Video-Quality-Assessment-And-Enhancement-For-Medical-Services-Norwegian-University-Of-Science-Technology-Ntnu=nLK80w-L7BGUYQAlkGUTnw.html</t>
         </is>
@@ -1971,10 +2389,15 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
+          <t>about 1 month ago</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
           <t>PhD Studentship Opportunity: Deep learning for increasing human sketch expressivity</t>
         </is>
       </c>
-      <c r="C91" t="inlineStr">
+      <c r="D91" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-United-Kingdom/Ph-D-Studentship-Opportunity-Deep-Learning-For-Increasing-Human-Sketch-Expressivity-University-Of-Surrey=QIi02Ny27BGUYQAlkGUTnw.html</t>
         </is>
@@ -1988,10 +2411,15 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
+          <t>about 2 months ago</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
           <t>PhD Studentship Opportunity: Detection of Peripheral Artery Disease from Photoplethysmography Signals Using Machine Learning</t>
         </is>
       </c>
-      <c r="C92" t="inlineStr">
+      <c r="D92" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-United-Kingdom/Ph-D-Studentship-Opportunity-Detection-Of-Peripheral-Artery-Disease-From-Photoplethysmography-Signals-Using-Machine-Learning-University-Of-Surrey=S22-7Omu7BGUYQAlkGUTnw.html</t>
         </is>
@@ -2005,10 +2433,15 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
+          <t>3 days ago</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
           <t>PhD Studentship Opportunity: Machine Learning for Audio with Applications for Health and Wellbeing</t>
         </is>
       </c>
-      <c r="C93" t="inlineStr">
+      <c r="D93" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-United-Kingdom/Ph-D-Studentship-Opportunity-Machine-Learning-For-Audio-With-Applications-For-Health-And-Wellbeing-University-Of-Surrey=S8g0ej-R7BGUYQAlkGUTnw.html</t>
         </is>
@@ -2022,10 +2455,15 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
+          <t>18 days ago</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
           <t>PhD Studentship Opportunity: Representation Learning from Fewer Labels</t>
         </is>
       </c>
-      <c r="C94" t="inlineStr">
+      <c r="D94" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-United-Kingdom/Ph-D-Studentship-Opportunity-Representation-Learning-From-Fewer-Labels-University-Of-Surrey=dPWFBUTF7BGUYQAlkGUTnw.html</t>
         </is>
@@ -2039,10 +2477,15 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
+          <t>4 days ago</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
           <t>PhD Studentship in Formal Methods for Safe Artificial Intelligence</t>
         </is>
       </c>
-      <c r="C95" t="inlineStr">
+      <c r="D95" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-United-Kingdom/Ph-D-Studentship-In-Formal-Methods-For-Safe-Artificial-Intelligence-University-Of-Birmingham=8myJpT-R7BGUYQAlkGUTnw.html</t>
         </is>
@@ -2056,10 +2499,15 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
+          <t>about 2 months ago</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
           <t>PhD Studentship: Deep Learning for Hydrodynamic Modelling of Wave to Soft-Structure Interaction.</t>
         </is>
       </c>
-      <c r="C96" t="inlineStr">
+      <c r="D96" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-United-Kingdom/Ph-D-Studentship-Deep-Learning-For-Hydrodynamic-Modelling-Of-Wave-To-Soft-Structure-Interaction-The-University-Of-Manchester=prT_Diel7BGUYAAlkGUTnw.html</t>
         </is>
@@ -2073,10 +2521,15 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
+          <t>2 months ago</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
           <t>PhD Studentship: My World/Netflix: Deep Video Coding for AOM/AV2</t>
         </is>
       </c>
-      <c r="C97" t="inlineStr">
+      <c r="D97" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-United-Kingdom/Ph-D-Studentship-My-World-Netflix-Deep-Video-Coding-For-Aom-Av2-University-Of-Bristol=QhADjmib7BGUYAAlkGUTnw.html</t>
         </is>
@@ -2088,12 +2541,13 @@
           <t>United Kingdom</t>
         </is>
       </c>
-      <c r="B98" t="inlineStr">
+      <c r="B98" t="inlineStr"/>
+      <c r="C98" t="inlineStr">
         <is>
           <t>PhD studentship in Formal Methods for Safe Artificial Intelligence</t>
         </is>
       </c>
-      <c r="C98" t="inlineStr">
+      <c r="D98" t="inlineStr">
         <is>
           <t>https://www.findaphd.com/phds/project/phd-studentship-in-formal-methods-for-safe-artificial-intelligence/?p144523</t>
         </is>
@@ -2107,10 +2561,15 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
+          <t>23 days ago</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
           <t>PhD studentships in Efficient and Reliable Probabilistic Machine Learning</t>
         </is>
       </c>
-      <c r="C99" t="inlineStr">
+      <c r="D99" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-United-Kingdom/Ph-D-Studentships-In-Efficient-And-Reliable-Probabilistic-Machine-Learning-The-University-Of-Edinburgh=J8gLuR-B7BGUYQAlkGUTnw.html</t>
         </is>
@@ -2122,12 +2581,13 @@
           <t>United Kingdom</t>
         </is>
       </c>
-      <c r="B100" t="inlineStr">
+      <c r="B100" t="inlineStr"/>
+      <c r="C100" t="inlineStr">
         <is>
           <t>Probabilistic programming for discovery of sustainable materials</t>
         </is>
       </c>
-      <c r="C100" t="inlineStr">
+      <c r="D100" t="inlineStr">
         <is>
           <t>https://www.findaphd.com/phds/project/probabilistic-programming-for-discovery-of-sustainable-materials/?p139631</t>
         </is>
@@ -2141,10 +2601,15 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
+          <t>25 days ago</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
           <t>Research Assistant under Division of Science, Computer Science, Prof. Djellel Difallah</t>
         </is>
       </c>
-      <c r="C101" t="inlineStr">
+      <c r="D101" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/jobs-in-United-Kingdom/Research-Assistant-Under-Division-Of-Science-Computer-Science-Prof-Djellel-Difallah-New-York-University-Abu-Dhabi=k9Djv-2-7BGUYQAlkGUTnw.html</t>
         </is>
@@ -2158,10 +2623,15 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
+          <t>8 days ago</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
           <t>Research Assistant/Associate in Computational Neuroscience (Fixed Term)</t>
         </is>
       </c>
-      <c r="C102" t="inlineStr">
+      <c r="D102" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/jobs-in-United-Kingdom/Research-Assistant-Associate-In-Computational-Neuroscience-Fixed-Term-University-Of-Cambridge=duYVLObN7BGUYQAlkGUTnw.html</t>
         </is>
@@ -2175,10 +2645,15 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
+          <t>3 months ago</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
           <t>Research Associate</t>
         </is>
       </c>
-      <c r="C103" t="inlineStr">
+      <c r="D103" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/jobs-in-United-Kingdom/Anchor-Anchor-Research-Associate-Anchor-King-s-College-London=2Lvw_R2F7BGUYAAlkGUTnw.html</t>
         </is>
@@ -2192,10 +2667,15 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
+          <t>21 days ago</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
           <t>Research Associate (Fixed Term)</t>
         </is>
       </c>
-      <c r="C104" t="inlineStr">
+      <c r="D104" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/jobs-in-United-Kingdom/Research-Associate-Fixed-Term-University-Of-Cambridge=ahXh-rXD7BGUYQAlkGUTnw.html</t>
         </is>
@@ -2209,10 +2689,15 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
+          <t>1 day ago</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
           <t>Research Associate in Image Analysis</t>
         </is>
       </c>
-      <c r="C105" t="inlineStr">
+      <c r="D105" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/jobs-in-United-Kingdom/Research-Associate-In-Image-Analysis-Imperial-College-London=61LXqezQ7BGUYQAlkGUTnw.html</t>
         </is>
@@ -2224,12 +2709,13 @@
           <t>United Kingdom</t>
         </is>
       </c>
-      <c r="B106" t="inlineStr">
+      <c r="B106" t="inlineStr"/>
+      <c r="C106" t="inlineStr">
         <is>
           <t>Security of Medical Cyber-Physical Systems</t>
         </is>
       </c>
-      <c r="C106" t="inlineStr">
+      <c r="D106" t="inlineStr">
         <is>
           <t>https://www.findaphd.com/phds/project/security-of-medical-cyber-physical-systems/?p137923</t>
         </is>
@@ -2243,10 +2729,15 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
+          <t>about 24 hours ago</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
           <t>Studentship: Sensor Fusion for Sustainable Process Technology</t>
         </is>
       </c>
-      <c r="C107" t="inlineStr">
+      <c r="D107" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-United-Kingdom/Studentship-Sensor-Fusion-For-Sustainable-Process-Technology-University-Of-Nottingham=JLnqgL-R7BGUYQAlkGUTnw.html</t>
         </is>
@@ -2260,10 +2751,15 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
+          <t>3 days ago</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
           <t>Studentship: Sensor Fusion for Sustainable Process Technology</t>
         </is>
       </c>
-      <c r="C108" t="inlineStr">
+      <c r="D108" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-United-Kingdom/Studentship-Sensor-Fusion-For-Sustainable-Process-Technology-University-Of-Nottingham=iXYAKgzS7BGUYQAlkGUTnw.html</t>
         </is>
@@ -2275,12 +2771,13 @@
           <t>United Kingdom</t>
         </is>
       </c>
-      <c r="B109" t="inlineStr">
+      <c r="B109" t="inlineStr"/>
+      <c r="C109" t="inlineStr">
         <is>
           <t>XAI Health: Explainability for Artificial Intelligence (AI) in the Healthcare Sector</t>
         </is>
       </c>
-      <c r="C109" t="inlineStr">
+      <c r="D109" t="inlineStr">
         <is>
           <t>https://www.findaphd.com/phds/project/xai-health-explainability-for-artificial-intelligence-ai-in-the-healthcare-sector/?p144424</t>
         </is>
@@ -2294,10 +2791,15 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
+          <t>5 days ago</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
           <t>Faculty Position in Mathematics of Earth Hazards at SMU</t>
         </is>
       </c>
-      <c r="C110" t="inlineStr">
+      <c r="D110" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-United-States/Faculty-Position-In-Mathematics-Of-Earth-Hazards-At-Smu-Southern-Methodist-University=W2CmB87O7BGUYQAlkGUTnw.html</t>
         </is>
@@ -2311,10 +2813,15 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
+          <t>about 12 hours ago</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
           <t>POSTDOCTORAL SCHOLAR-CARDIAC MRI DEEP LEARNING</t>
         </is>
       </c>
-      <c r="C111" t="inlineStr">
+      <c r="D111" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/jobs-in-United-States/Postdoctoral-Scholar-Cardiac-Mri-Deep-Learning-The-University-Of-Iowa=ICt5nM2U7BGUYAAlkGUTnw.html</t>
         </is>
@@ -2328,10 +2835,15 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
+          <t>about 5 hours ago</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
           <t>Ph.D. student in flash drought and climate</t>
         </is>
       </c>
-      <c r="C112" t="inlineStr">
+      <c r="D112" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-United-States/Ph-D-Student-In-Flash-Drought-And-Climate-Auburn-University=YnlpW-XE7BGUYQAlkGUTnw.html</t>
         </is>
@@ -2345,10 +2857,15 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
+          <t>about 1 month ago</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
           <t>PhD position in Electrical and Computer Engineering with focus on Deep Learning and Machine Learning</t>
         </is>
       </c>
-      <c r="C113" t="inlineStr">
+      <c r="D113" t="inlineStr">
         <is>
           <t>https://scholarshipdb.net/scholarships-in-United-States/Ph-D-Position-In-Electrical-And-Computer-Engineering-With-Focus-On-Deep-Learning-And-Machine-Learning-The-University-Of-Alabama=Jh9gDcocYO84MoUbvpyAk5.html</t>
         </is>

</xml_diff>